<commit_message>
Notes taken on 6/20/22
</commit_message>
<xml_diff>
--- a/pandas/4_read_write_to_excel/stocks_weather.xlsx
+++ b/pandas/4_read_write_to_excel/stocks_weather.xlsx
@@ -17,18 +17,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
+    <t>eps</t>
+  </si>
+  <si>
+    <t>pe</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
     <t>tickers</t>
   </si>
   <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>pe</t>
-  </si>
-  <si>
-    <t>eps</t>
-  </si>
-  <si>
     <t>GOOGL</t>
   </si>
   <si>
@@ -41,10 +41,10 @@
     <t>day</t>
   </si>
   <si>
+    <t>event</t>
+  </si>
+  <si>
     <t>temperature</t>
-  </si>
-  <si>
-    <t>event</t>
   </si>
   <si>
     <t>1/1/2017</t>
@@ -444,51 +444,51 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>27.82</v>
+      </c>
+      <c r="C2">
+        <v>30.37</v>
+      </c>
+      <c r="D2">
+        <v>845</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2">
-        <v>845</v>
-      </c>
-      <c r="D2">
-        <v>30.37</v>
-      </c>
-      <c r="E2">
-        <v>27.82</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>4.61</v>
+      </c>
+      <c r="C3">
+        <v>14.26</v>
+      </c>
+      <c r="D3">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3">
-        <v>65</v>
-      </c>
-      <c r="D3">
-        <v>14.26</v>
-      </c>
-      <c r="E3">
-        <v>4.61</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>2.12</v>
+      </c>
+      <c r="C4">
+        <v>30.97</v>
+      </c>
+      <c r="D4">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4">
-        <v>64</v>
-      </c>
-      <c r="D4">
-        <v>30.97</v>
-      </c>
-      <c r="E4">
-        <v>2.12</v>
       </c>
     </row>
   </sheetData>
@@ -522,11 +522,11 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
         <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -536,11 +536,11 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
         <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -550,11 +550,11 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
         <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>